<commit_message>
a preliminary map added
</commit_message>
<xml_diff>
--- a/Geocoding ALL.xlsx
+++ b/Geocoding ALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaosiyue/Documents/Columbia MSPH/Spring 2023/P9300 - Capstone/ehs_capstone_nycdoh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4249B091-9702-634A-9607-4485E2A0DE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E1557E-95BD-2E41-8257-05683F51DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="500" windowWidth="21580" windowHeight="15920" xr2:uid="{239C503F-5ADE-E64C-9F21-63958588DC29}"/>
+    <workbookView xWindow="-40" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{239C503F-5ADE-E64C-9F21-63958588DC29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4201,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32AE7D6-8B55-0446-8960-92BAA3112B47}">
   <dimension ref="A1:F436"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
+      <selection activeCell="A397" sqref="A397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6052,7 +6052,7 @@
         <v>40.605549000000003</v>
       </c>
       <c r="E108" s="4">
-        <v>73.985397000000006</v>
+        <v>-73.985397000000006</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>